<commit_message>
Update: Add Keyword Function
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\tax\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
@@ -21,12 +16,7 @@
     <sheet name="mcu" sheetId="7" r:id="rId7"/>
     <sheet name="chip" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -51,6 +41,9 @@
     <t>Danh</t>
   </si>
   <si>
+    <t>DCU_2G(Sim800C)_4G(Sim7600CE)_SF80P20_Cover_1603757518</t>
+  </si>
+  <si>
     <t>LF_1pha_HT32F5 V1.3_03022021</t>
   </si>
   <si>
@@ -84,6 +77,9 @@
     <t>MODULE RF 1P SOC</t>
   </si>
   <si>
+    <t>MODULE RF 1P HOLTEK</t>
+  </si>
+  <si>
     <t>TỒN 30/06/2021</t>
   </si>
   <si>
@@ -115,12 +111,6 @@
   </si>
   <si>
     <t>HiSilicon</t>
-  </si>
-  <si>
-    <t>MODULE RF 1P HOLTEK</t>
-  </si>
-  <si>
-    <t>DCU_2G(Sim800C)_4G(Sim7600CE)_SF80P20_Cover_1603757518</t>
   </si>
 </sst>
 </file>
@@ -447,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +475,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -497,35 +487,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
@@ -533,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -541,22 +531,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -568,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -576,22 +566,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -603,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -611,7 +601,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -631,17 +621,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -661,22 +651,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -696,17 +686,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>